<commit_message>
brief rearrangement for results and conclusion
</commit_message>
<xml_diff>
--- a/event_study_240_day_without_10_days_gap/event_study/mentioned_stock.xlsx
+++ b/event_study_240_day_without_10_days_gap/event_study/mentioned_stock.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Python Quant\TrumpTweetsPrivate\event_study\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lance\Documents\GitHub\TrumpTweetsProject\event_study_240_day_without_10_days_gap\event_study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A582AAD-1FD9-419F-BC82-BC96CBE6B63C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72C3952-84BD-4AB4-9D63-F0FC785DF97D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20715" windowHeight="13275" xr2:uid="{7878AB7C-8233-0E4A-9B23-CE8563D81F18}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17184" windowHeight="11328" xr2:uid="{7878AB7C-8233-0E4A-9B23-CE8563D81F18}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">table!$D$1:$D$80</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -980,27 +980,27 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1014,7 +1014,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1046,9 +1046,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1074,11 +1074,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -1540,13 +1540,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1601,13 +1601,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2199,20 +2199,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E4B5DEB-6ED9-3A48-9AFB-493EBF1260C4}">
   <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="23.375" customWidth="1"/>
-    <col min="2" max="2" width="15.625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="17"/>
-    <col min="5" max="5" width="37.875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.3984375" customWidth="1"/>
+    <col min="2" max="2" width="15.59765625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="10.8984375" style="17"/>
+    <col min="5" max="5" width="37.8984375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="17.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -2229,109 +2229,109 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
-        <v>43544.86922453704</v>
+    <row r="2" spans="1:5">
+      <c r="A2" s="14">
+        <v>43193.580289351848</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>127</v>
+        <v>188</v>
       </c>
       <c r="D2" s="12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
-        <v>43541.935729166667</v>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="14">
+        <v>43098.544548611113</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>209</v>
+        <v>38</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>128</v>
+        <v>188</v>
       </c>
       <c r="D3" s="12">
         <v>-1</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
-        <v>43538.679629629631</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="14">
+        <v>42963.425520833327</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>129</v>
+        <v>188</v>
       </c>
       <c r="D4" s="12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
-        <v>43523.389178240737</v>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="15">
+        <v>42941.108530092592</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>130</v>
+        <v>188</v>
       </c>
       <c r="D5" s="12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
-        <v>43433.484189814822</v>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="15">
+        <v>42937.147048611107</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>209</v>
+        <v>38</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>128</v>
+        <v>188</v>
       </c>
       <c r="D6" s="12">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
-        <v>43431.795590277783</v>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="14">
+        <v>43000.746516203697</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D7" s="12">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="14">
         <v>43322.949826388889</v>
       </c>
@@ -2348,143 +2348,143 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="14">
-        <v>43306.027268518519</v>
+        <v>43117.978125000001</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D9" s="12">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
-        <v>43306.027268518519</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="15">
+        <v>42710.369444444441</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>142</v>
+        <v>207</v>
       </c>
       <c r="D10" s="12">
         <v>-1</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
-        <v>43300.432800925933</v>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="15">
+        <v>42726.726388888892</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>36</v>
+        <v>197</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>144</v>
+        <v>207</v>
       </c>
       <c r="D11" s="12">
         <v>1</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="14">
-        <v>43291.942685185182</v>
+        <v>43041.856458333343</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>37</v>
+        <v>195</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="D12" s="12">
         <v>1</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="14">
-        <v>43290.714224537027</v>
+        <v>43124.499282407407</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>37</v>
+        <v>204</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="D13" s="12">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
-        <v>43277.484618055547</v>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="15">
+        <v>42937.147048611107</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>136</v>
+        <v>189</v>
       </c>
       <c r="D14" s="12">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
-        <v>43193.580289351848</v>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="15">
+        <v>42800.679861111108</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>38</v>
+        <v>202</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>188</v>
+        <v>221</v>
       </c>
       <c r="D15" s="12">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
-        <v>43165.546620370369</v>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="13">
+        <v>43523.389178240737</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D16" s="12">
         <v>1</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="14">
         <v>43128.554548611108</v>
       </c>
@@ -2501,276 +2501,276 @@
         <v>214</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="14">
-        <v>43124.499282407407</v>
+        <v>43112.120196759257</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>205</v>
+        <v>40</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D18" s="12">
         <v>1</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
-        <v>43124.499282407407</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="15">
+        <v>42744.593171296299</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>194</v>
+        <v>40</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D19" s="12">
         <v>1</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="14">
-        <v>43124.499282407407</v>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="13">
+        <v>43544.86922453704</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>204</v>
+        <v>34</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="D20" s="12">
         <v>1</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
-        <v>43117.978125000001</v>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="15">
+        <v>42822.441689814812</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>190</v>
+        <v>34</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D21" s="12">
         <v>1</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="14">
-        <v>43112.120196759257</v>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="15">
+        <v>42744.594837962963</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D22" s="12">
         <v>1</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="14">
-        <v>43111.186828703707</v>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="15">
+        <v>42739.554965277777</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D23" s="12">
         <v>1</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="14">
-        <v>43098.544548611113</v>
+        <v>236</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="15">
+        <v>42691.910416666666</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>188</v>
+        <v>127</v>
       </c>
       <c r="D24" s="12">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="14">
-        <v>43041.856458333343</v>
+        <v>43165.546620370369</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>195</v>
+        <v>39</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D25" s="12">
         <v>1</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="14">
-        <v>43000.746516203697</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="15">
+        <v>42760.032604166663</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>203</v>
+        <v>228</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D26" s="12">
         <v>1</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="14">
-        <v>42963.425520833327</v>
+        <v>229</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="15">
+        <v>42752.746967592589</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>38</v>
+        <v>228</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>188</v>
+        <v>128</v>
       </c>
       <c r="D27" s="12">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="14">
-        <v>42961.538043981483</v>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="15">
+        <v>42738.520891203712</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>124</v>
+        <v>228</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D28" s="12">
         <v>-1</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="15">
-        <v>42941.108530092592</v>
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="13">
+        <v>43541.935729166667</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>38</v>
+        <v>209</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>188</v>
+        <v>128</v>
       </c>
       <c r="D29" s="12">
         <v>-1</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="15">
-        <v>42937.147048611107</v>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="13">
+        <v>43433.484189814822</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>124</v>
+        <v>209</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D30" s="12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="15">
-        <v>42937.147048611107</v>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="13">
+        <v>43431.795590277783</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>37</v>
+        <v>209</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D31" s="12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="15">
-        <v>42937.147048611107</v>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="14">
+        <v>43277.484618055547</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>189</v>
+        <v>136</v>
       </c>
       <c r="D32" s="12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="15">
-        <v>42937.147048611107</v>
+        <v>42774.807326388887</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>38</v>
+        <v>223</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>188</v>
+        <v>224</v>
       </c>
       <c r="D33" s="12">
         <v>1</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="H33" s="9"/>
       <c r="I33" s="10"/>
@@ -2778,21 +2778,21 @@
       <c r="K33" s="9"/>
       <c r="L33" s="6"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="15">
-        <v>42862.957488425927</v>
+    <row r="34" spans="1:12">
+      <c r="A34" s="14">
+        <v>43124.499282407407</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>187</v>
+        <v>133</v>
       </c>
       <c r="D34" s="12">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
@@ -2802,21 +2802,21 @@
       <c r="K34" s="9"/>
       <c r="L34" s="6"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12">
       <c r="A35" s="15">
-        <v>42822.441689814812</v>
+        <v>42716.601388888892</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>34</v>
+        <v>198</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>127</v>
+        <v>186</v>
       </c>
       <c r="D35" s="12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
@@ -2825,21 +2825,21 @@
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12">
       <c r="A36" s="15">
-        <v>42800.679861111108</v>
+        <v>42726.726388888892</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="D36" s="12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>222</v>
+        <v>241</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
@@ -2848,42 +2848,42 @@
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
     </row>
-    <row r="37" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="15">
-        <v>42774.807326388887</v>
+    <row r="37" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A37" s="14">
+        <v>42961.538043981483</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>223</v>
+        <v>124</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>224</v>
+        <v>135</v>
       </c>
       <c r="D37" s="12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>225</v>
+        <v>125</v>
       </c>
       <c r="H37" s="9"/>
       <c r="I37" s="10"/>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12">
       <c r="A38" s="15">
-        <v>42774.660428240742</v>
+        <v>42937.147048611107</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>226</v>
+        <v>124</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>185</v>
+        <v>135</v>
       </c>
       <c r="D38" s="12">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
@@ -2892,42 +2892,42 @@
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="A39" s="15">
-        <v>42760.032604166663</v>
+        <v>42774.660428240742</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>128</v>
+        <v>185</v>
       </c>
       <c r="D39" s="12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H39" s="9"/>
       <c r="I39" s="10"/>
       <c r="J39" s="9"/>
       <c r="K39" s="6"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="15">
-        <v>42752.746967592589</v>
+    <row r="40" spans="1:12">
+      <c r="A40" s="14">
+        <v>43300.432800925933</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>228</v>
+        <v>36</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="D40" s="12">
         <v>1</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>230</v>
+        <v>44</v>
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
@@ -2936,21 +2936,21 @@
       <c r="J40" s="9"/>
       <c r="K40" s="6"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="15">
-        <v>42752.746967592589</v>
+    <row r="41" spans="1:12">
+      <c r="A41" s="14">
+        <v>43291.942685185182</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>231</v>
+        <v>37</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>232</v>
+        <v>132</v>
       </c>
       <c r="D41" s="12">
         <v>1</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>230</v>
+        <v>44</v>
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
@@ -2960,21 +2960,21 @@
       <c r="K41" s="9"/>
       <c r="L41" s="9"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="15">
-        <v>42744.594837962963</v>
+    <row r="42" spans="1:12">
+      <c r="A42" s="14">
+        <v>43290.714224537027</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D42" s="12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>233</v>
+        <v>45</v>
       </c>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
@@ -2984,42 +2984,42 @@
       <c r="K42" s="6"/>
       <c r="L42" s="9"/>
     </row>
-    <row r="43" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="16.2" customHeight="1">
       <c r="A43" s="15">
-        <v>42744.593171296299</v>
+        <v>42937.147048611107</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D43" s="12">
         <v>1</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="H43" s="9"/>
       <c r="I43" s="10"/>
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12">
       <c r="A44" s="15">
-        <v>42740.760069444441</v>
+        <v>42862.957488425927</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>35</v>
+        <v>196</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>129</v>
+        <v>187</v>
       </c>
       <c r="D44" s="12">
         <v>-1</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
@@ -3029,126 +3029,126 @@
       <c r="K44" s="9"/>
       <c r="L44" s="9"/>
     </row>
-    <row r="45" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="16.2" customHeight="1">
       <c r="A45" s="15">
-        <v>42739.554965277777</v>
+        <v>42706.92083333333</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>34</v>
+        <v>196</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>127</v>
+        <v>187</v>
       </c>
       <c r="D45" s="12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="15">
-        <v>42738.520891203712</v>
+        <v>238</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="16.2" customHeight="1">
+      <c r="A46" s="14">
+        <v>43306.027268518519</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>228</v>
+        <v>192</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="D46" s="12">
         <v>-1</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="16.2" customHeight="1">
       <c r="A47" s="15">
-        <v>42706.92083333333</v>
+        <v>42710.590277777781</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>187</v>
+        <v>247</v>
       </c>
       <c r="D47" s="12">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="15">
-        <v>42710.369444444441</v>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="16.2" customHeight="1">
+      <c r="A48" s="13">
+        <v>43538.679629629631</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>197</v>
+        <v>35</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>207</v>
+        <v>129</v>
       </c>
       <c r="D48" s="12">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="15">
-        <v>42716.601388888892</v>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="16.2" customHeight="1">
+      <c r="A49" s="14">
+        <v>43111.186828703707</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>198</v>
+        <v>35</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>186</v>
+        <v>129</v>
       </c>
       <c r="D49" s="12">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" s="15">
-        <v>42726.726388888892</v>
+        <v>42740.760069444441</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>198</v>
+        <v>35</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>186</v>
+        <v>129</v>
       </c>
       <c r="D50" s="12">
         <v>-1</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="15">
-        <v>42691.910416666666</v>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" s="14">
+        <v>43306.027268518519</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>34</v>
+        <v>191</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="D51" s="12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
       <c r="A52" s="15">
         <v>42698.425000000003</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12">
       <c r="A53" s="15">
         <v>42703.944444444445</v>
       </c>
@@ -3182,53 +3182,53 @@
         <v>244</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12">
       <c r="A54" s="15">
-        <v>42710.590277777781</v>
+        <v>42752.746967592589</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>200</v>
+        <v>231</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="D54" s="12">
         <v>1</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="L54" s="9"/>
     </row>
-    <row r="55" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="15">
-        <v>42726.726388888892</v>
+    <row r="55" spans="1:12" ht="16.2" customHeight="1">
+      <c r="A55" s="14">
+        <v>43124.499282407407</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>207</v>
+        <v>138</v>
       </c>
       <c r="D55" s="12">
         <v>1</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="L55" s="9"/>
     </row>
-    <row r="56" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="16.2" customHeight="1">
       <c r="B56" s="16"/>
       <c r="C56" s="16"/>
       <c r="L56" s="9"/>
     </row>
-    <row r="57" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="16.2" customHeight="1">
       <c r="B57" s="16"/>
       <c r="C57" s="16"/>
       <c r="L57" s="6"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12">
       <c r="B58" s="16"/>
       <c r="C58" s="16"/>
       <c r="F58" s="6"/>
@@ -3239,7 +3239,7 @@
       <c r="K58" s="6"/>
       <c r="L58" s="6"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12">
       <c r="B59" s="16"/>
       <c r="C59" s="16"/>
       <c r="F59" s="6"/>
@@ -3250,7 +3250,7 @@
       <c r="K59" s="6"/>
       <c r="L59" s="6"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12">
       <c r="B60" s="16"/>
       <c r="C60" s="16"/>
       <c r="F60" s="6"/>
@@ -3261,7 +3261,7 @@
       <c r="K60" s="6"/>
       <c r="L60" s="6"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12">
       <c r="B61" s="16"/>
       <c r="C61" s="16"/>
       <c r="F61" s="6"/>
@@ -3272,7 +3272,7 @@
       <c r="K61" s="6"/>
       <c r="L61" s="6"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12">
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
       <c r="H62" s="6"/>
@@ -3281,7 +3281,7 @@
       <c r="K62" s="6"/>
       <c r="L62" s="6"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12">
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
       <c r="H63" s="6"/>
@@ -3290,7 +3290,7 @@
       <c r="K63" s="6"/>
       <c r="L63" s="6"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12">
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
       <c r="H64" s="6"/>
@@ -3299,7 +3299,7 @@
       <c r="K64" s="6"/>
       <c r="L64" s="6"/>
     </row>
-    <row r="65" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="6:12">
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
       <c r="H65" s="6"/>
@@ -3308,7 +3308,7 @@
       <c r="K65" s="6"/>
       <c r="L65" s="6"/>
     </row>
-    <row r="66" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="6:12">
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
       <c r="H66" s="6"/>
@@ -3317,7 +3317,7 @@
       <c r="K66" s="6"/>
       <c r="L66" s="6"/>
     </row>
-    <row r="67" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="6:12">
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
       <c r="H67" s="6"/>
@@ -3326,7 +3326,7 @@
       <c r="K67" s="6"/>
       <c r="L67" s="6"/>
     </row>
-    <row r="68" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="6:12">
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
       <c r="H68" s="6"/>
@@ -3335,7 +3335,7 @@
       <c r="K68" s="6"/>
       <c r="L68" s="6"/>
     </row>
-    <row r="69" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="6:12">
       <c r="F69" s="6"/>
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
@@ -3344,7 +3344,7 @@
       <c r="K69" s="6"/>
       <c r="L69" s="6"/>
     </row>
-    <row r="70" spans="6:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="6:12">
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
       <c r="H70" s="6"/>
@@ -3353,48 +3353,48 @@
       <c r="K70" s="6"/>
       <c r="L70" s="6"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7">
       <c r="E83"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7">
       <c r="E84"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7">
       <c r="E85"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7">
       <c r="E86"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7">
       <c r="E87"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7">
       <c r="E88"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7">
       <c r="E89"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7">
       <c r="E90"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7">
       <c r="E91"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7">
       <c r="E92"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7">
       <c r="E93"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7">
       <c r="E94"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7">
       <c r="C95" s="18"/>
       <c r="D95" s="8"/>
       <c r="E95"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7">
       <c r="A96" s="4"/>
       <c r="B96" s="18"/>
       <c r="C96" s="18"/>
@@ -3402,7 +3402,7 @@
       <c r="E96"/>
       <c r="G96" s="4"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7">
       <c r="A97" s="4"/>
       <c r="B97" s="18"/>
       <c r="C97" s="18"/>
@@ -3411,7 +3411,7 @@
       <c r="F97" s="4"/>
       <c r="G97" s="4"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7">
       <c r="A98" s="4"/>
       <c r="B98" s="18"/>
       <c r="C98" s="18"/>
@@ -3419,25 +3419,28 @@
       <c r="E98"/>
       <c r="G98" s="4"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7">
       <c r="E99"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7">
       <c r="E100"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7">
       <c r="E101"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7">
       <c r="E102"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7">
       <c r="E103"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7">
       <c r="E104"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E104">
+    <sortCondition ref="B2:B104"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3452,13 +3455,13 @@
       <selection activeCell="B29" sqref="B29:G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6"/>
   <cols>
     <col min="2" max="2" width="18" style="6" customWidth="1"/>
-    <col min="4" max="4" width="20.625" customWidth="1"/>
+    <col min="4" max="4" width="20.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7">
       <c r="B1" s="6" t="s">
         <v>6</v>
       </c>
@@ -3478,7 +3481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7">
       <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
@@ -3498,7 +3501,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7">
       <c r="B3" s="6" t="s">
         <v>11</v>
       </c>
@@ -3518,7 +3521,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7">
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -3538,7 +3541,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7">
       <c r="B5" s="6" t="s">
         <v>26</v>
       </c>
@@ -3558,7 +3561,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7">
       <c r="B6" s="6" t="s">
         <v>30</v>
       </c>
@@ -3578,7 +3581,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7">
       <c r="B7" s="6" t="s">
         <v>17</v>
       </c>
@@ -3598,7 +3601,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7">
       <c r="B8" s="2" t="s">
         <v>51</v>
       </c>
@@ -3618,7 +3621,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7">
       <c r="B9" s="2" t="s">
         <v>54</v>
       </c>
@@ -3638,7 +3641,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7">
       <c r="B10" s="2" t="s">
         <v>54</v>
       </c>
@@ -3654,7 +3657,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7">
       <c r="B11" s="2" t="s">
         <v>57</v>
       </c>
@@ -3674,7 +3677,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7">
       <c r="B12" s="2" t="s">
         <v>61</v>
       </c>
@@ -3694,7 +3697,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7">
       <c r="B13" s="2" t="s">
         <v>65</v>
       </c>
@@ -3714,7 +3717,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7">
       <c r="B14" s="2" t="s">
         <v>69</v>
       </c>
@@ -3734,7 +3737,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7">
       <c r="B15" s="2" t="s">
         <v>73</v>
       </c>
@@ -3754,7 +3757,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7">
       <c r="B16" s="2" t="s">
         <v>77</v>
       </c>
@@ -3774,7 +3777,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7">
       <c r="B17" s="2" t="s">
         <v>81</v>
       </c>
@@ -3794,7 +3797,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7">
       <c r="B18" s="2" t="s">
         <v>84</v>
       </c>
@@ -3814,7 +3817,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7">
       <c r="B19" s="2" t="s">
         <v>84</v>
       </c>
@@ -3830,7 +3833,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7">
       <c r="B20" s="2" t="s">
         <v>84</v>
       </c>
@@ -3846,7 +3849,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7">
       <c r="B21" s="2" t="s">
         <v>87</v>
       </c>
@@ -3866,7 +3869,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7">
       <c r="B22" s="2" t="s">
         <v>90</v>
       </c>
@@ -3886,7 +3889,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7">
       <c r="B23" s="2" t="s">
         <v>92</v>
       </c>
@@ -3906,7 +3909,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7">
       <c r="B24" s="2" t="s">
         <v>101</v>
       </c>
@@ -3926,7 +3929,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7">
       <c r="B25" s="2" t="s">
         <v>105</v>
       </c>
@@ -3946,7 +3949,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7">
       <c r="B26" s="2" t="s">
         <v>109</v>
       </c>
@@ -3966,7 +3969,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7">
       <c r="B27" s="2" t="s">
         <v>113</v>
       </c>
@@ -3986,7 +3989,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7">
       <c r="B28" s="2" t="s">
         <v>117</v>
       </c>
@@ -4006,7 +4009,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7">
       <c r="B29" s="2" t="s">
         <v>145</v>
       </c>
@@ -4026,7 +4029,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7">
       <c r="B30" s="2" t="s">
         <v>147</v>
       </c>
@@ -4046,7 +4049,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7">
       <c r="B31" s="2" t="s">
         <v>151</v>
       </c>
@@ -4066,7 +4069,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7">
       <c r="B32" s="2" t="s">
         <v>155</v>
       </c>
@@ -4086,7 +4089,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7">
       <c r="B33" s="2" t="s">
         <v>158</v>
       </c>
@@ -4106,7 +4109,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7">
       <c r="B34" s="2" t="s">
         <v>162</v>
       </c>
@@ -4126,7 +4129,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7">
       <c r="B35" s="2" t="s">
         <v>165</v>
       </c>
@@ -4146,7 +4149,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7">
       <c r="B36" s="2" t="s">
         <v>169</v>
       </c>
@@ -4166,7 +4169,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7">
       <c r="B37" s="2" t="s">
         <v>172</v>
       </c>
@@ -4186,7 +4189,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7">
       <c r="B38" s="2" t="s">
         <v>176</v>
       </c>
@@ -4206,7 +4209,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7">
       <c r="B39" s="2" t="s">
         <v>178</v>
       </c>
@@ -4226,7 +4229,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7">
       <c r="B40" s="2" t="s">
         <v>180</v>
       </c>
@@ -4246,7 +4249,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7">
       <c r="B41" s="2" t="s">
         <v>182</v>
       </c>

</xml_diff>